<commit_message>
Se actualiza  seguimiento 2 semana de sprint 1
</commit_message>
<xml_diff>
--- a/SPRINT 1/1-Planificacion/Pila del Sprint/Pila General del Sprint 1.xlsx
+++ b/SPRINT 1/1-Planificacion/Pila del Sprint/Pila General del Sprint 1.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18229"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Juan Pablo\Documents\Proyecto de Grado JP\SPRINT 1\1-Planificacion\Pila del Sprint\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\ACER-PC\Documents\Proyecto de Grado JP\Proyecto\SPRINT 1\1-Planificacion\Pila del Sprint\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -650,6 +650,27 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -662,12 +683,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -677,23 +692,8 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -978,7 +978,7 @@
   <dimension ref="B1:P46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="M33" sqref="M33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -1000,91 +1000,91 @@
   <sheetData>
     <row r="1" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33"/>
-      <c r="K2" s="33"/>
-      <c r="L2" s="33"/>
-      <c r="M2" s="33"/>
-      <c r="N2" s="33"/>
-      <c r="O2" s="33"/>
-      <c r="P2" s="33"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
+      <c r="L2" s="19"/>
+      <c r="M2" s="19"/>
+      <c r="N2" s="19"/>
+      <c r="O2" s="19"/>
+      <c r="P2" s="19"/>
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="33"/>
-      <c r="I3" s="33"/>
-      <c r="J3" s="33"/>
-      <c r="K3" s="33"/>
-      <c r="L3" s="33"/>
-      <c r="M3" s="33"/>
-      <c r="N3" s="33"/>
-      <c r="O3" s="33"/>
-      <c r="P3" s="33"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
+      <c r="K3" s="19"/>
+      <c r="L3" s="19"/>
+      <c r="M3" s="19"/>
+      <c r="N3" s="19"/>
+      <c r="O3" s="19"/>
+      <c r="P3" s="19"/>
     </row>
     <row r="4" spans="2:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B5" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="28" t="s">
+      <c r="B5" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="28" t="s">
-        <v>2</v>
-      </c>
-      <c r="E5" s="28" t="s">
+      <c r="D5" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="G5" s="28" t="s">
+      <c r="F5" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="H5" s="19" t="s">
+      <c r="H5" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="I5" s="19" t="s">
+      <c r="I5" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="J5" s="22" t="s">
+      <c r="J5" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="K5" s="23" t="s">
+      <c r="K5" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="L5" s="25" t="s">
+      <c r="L5" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="M5" s="27" t="s">
+      <c r="M5" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="N5" s="28"/>
-      <c r="O5" s="28"/>
-      <c r="P5" s="29"/>
+      <c r="N5" s="22"/>
+      <c r="O5" s="22"/>
+      <c r="P5" s="33"/>
     </row>
     <row r="6" spans="2:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="31"/>
-      <c r="C6" s="32"/>
-      <c r="D6" s="32"/>
-      <c r="E6" s="32"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="32"/>
-      <c r="H6" s="20"/>
-      <c r="I6" s="21"/>
-      <c r="J6" s="20"/>
-      <c r="K6" s="24"/>
-      <c r="L6" s="26"/>
+      <c r="B6" s="21"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="27"/>
+      <c r="I6" s="28"/>
+      <c r="J6" s="27"/>
+      <c r="K6" s="25"/>
+      <c r="L6" s="31"/>
       <c r="M6" s="2" t="s">
         <v>11</v>
       </c>
@@ -1205,10 +1205,14 @@
       </c>
       <c r="L9" s="9">
         <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="M9" s="10"/>
-      <c r="N9" s="6"/>
+        <v>4</v>
+      </c>
+      <c r="M9" s="10">
+        <v>2</v>
+      </c>
+      <c r="N9" s="6">
+        <v>2</v>
+      </c>
       <c r="O9" s="6"/>
       <c r="P9" s="11"/>
     </row>
@@ -1243,10 +1247,14 @@
       </c>
       <c r="L10" s="9">
         <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="M10" s="10"/>
-      <c r="N10" s="6"/>
+        <v>4</v>
+      </c>
+      <c r="M10" s="10">
+        <v>2</v>
+      </c>
+      <c r="N10" s="6">
+        <v>2</v>
+      </c>
       <c r="O10" s="6"/>
       <c r="P10" s="11"/>
     </row>
@@ -1281,10 +1289,14 @@
       </c>
       <c r="L11" s="9">
         <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="M11" s="10"/>
-      <c r="N11" s="6"/>
+        <v>4</v>
+      </c>
+      <c r="M11" s="10">
+        <v>2</v>
+      </c>
+      <c r="N11" s="6">
+        <v>2</v>
+      </c>
       <c r="O11" s="6"/>
       <c r="P11" s="11"/>
     </row>
@@ -1319,9 +1331,11 @@
       </c>
       <c r="L12" s="9">
         <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M12" s="10">
         <v>10</v>
       </c>
-      <c r="M12" s="10"/>
       <c r="N12" s="6"/>
       <c r="O12" s="6"/>
       <c r="P12" s="11"/>
@@ -1357,10 +1371,14 @@
       </c>
       <c r="L13" s="9">
         <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="M13" s="14"/>
-      <c r="N13" s="12"/>
+        <v>0</v>
+      </c>
+      <c r="M13" s="14">
+        <v>2</v>
+      </c>
+      <c r="N13" s="12">
+        <v>2</v>
+      </c>
       <c r="O13" s="12"/>
       <c r="P13" s="15"/>
     </row>
@@ -1395,10 +1413,14 @@
       </c>
       <c r="L14" s="9">
         <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="M14" s="14"/>
-      <c r="N14" s="12"/>
+        <v>0</v>
+      </c>
+      <c r="M14" s="14">
+        <v>2</v>
+      </c>
+      <c r="N14" s="12">
+        <v>2</v>
+      </c>
       <c r="O14" s="12"/>
       <c r="P14" s="15"/>
     </row>
@@ -1435,7 +1457,9 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="M15" s="14"/>
+      <c r="M15" s="14">
+        <v>0</v>
+      </c>
       <c r="N15" s="12"/>
       <c r="O15" s="12"/>
       <c r="P15" s="15"/>
@@ -1458,13 +1482,19 @@
       <c r="J16" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="K16" s="12"/>
+      <c r="K16" s="12">
+        <v>4</v>
+      </c>
       <c r="L16" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M16" s="14"/>
-      <c r="N16" s="12"/>
+      <c r="M16" s="14">
+        <v>2</v>
+      </c>
+      <c r="N16" s="12">
+        <v>2</v>
+      </c>
       <c r="O16" s="12"/>
       <c r="P16" s="15"/>
     </row>
@@ -1495,14 +1525,18 @@
         <v>64</v>
       </c>
       <c r="K17" s="12">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="L17" s="9">
         <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="M17" s="14"/>
-      <c r="N17" s="12"/>
+        <v>0</v>
+      </c>
+      <c r="M17" s="14">
+        <v>2</v>
+      </c>
+      <c r="N17" s="12">
+        <v>2</v>
+      </c>
       <c r="O17" s="12"/>
       <c r="P17" s="15"/>
     </row>
@@ -1526,13 +1560,19 @@
       <c r="J18" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="K18" s="12"/>
+      <c r="K18" s="12">
+        <v>4</v>
+      </c>
       <c r="L18" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M18" s="14"/>
-      <c r="N18" s="12"/>
+      <c r="M18" s="14">
+        <v>2</v>
+      </c>
+      <c r="N18" s="12">
+        <v>2</v>
+      </c>
       <c r="O18" s="12"/>
       <c r="P18" s="15"/>
     </row>
@@ -1558,13 +1598,19 @@
       <c r="J19" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="K19" s="12"/>
+      <c r="K19" s="12">
+        <v>4</v>
+      </c>
       <c r="L19" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M19" s="14"/>
-      <c r="N19" s="12"/>
+      <c r="M19" s="14">
+        <v>2</v>
+      </c>
+      <c r="N19" s="12">
+        <v>2</v>
+      </c>
       <c r="O19" s="12"/>
       <c r="P19" s="15"/>
     </row>
@@ -1595,13 +1641,14 @@
         <v>64</v>
       </c>
       <c r="K20" s="12">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="L20" s="9">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="M20" s="14"/>
+        <v>6</v>
+      </c>
+      <c r="M20" s="14">
+        <v>0</v>
+      </c>
       <c r="N20" s="12"/>
       <c r="O20" s="12"/>
       <c r="P20" s="15"/>
@@ -1639,7 +1686,9 @@
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="M21" s="14"/>
+      <c r="M21" s="14">
+        <v>0</v>
+      </c>
       <c r="N21" s="12"/>
       <c r="O21" s="12"/>
       <c r="P21" s="15"/>
@@ -1677,7 +1726,9 @@
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="M22" s="14"/>
+      <c r="M22" s="14">
+        <v>0</v>
+      </c>
       <c r="N22" s="12"/>
       <c r="O22" s="12"/>
       <c r="P22" s="15"/>
@@ -1713,9 +1764,11 @@
       </c>
       <c r="L23" s="9">
         <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="M23" s="14"/>
+        <v>0</v>
+      </c>
+      <c r="M23" s="14">
+        <v>4</v>
+      </c>
       <c r="N23" s="12"/>
       <c r="O23" s="12"/>
       <c r="P23" s="15"/>
@@ -1751,9 +1804,11 @@
       </c>
       <c r="L24" s="9">
         <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="M24" s="14"/>
+        <v>0</v>
+      </c>
+      <c r="M24" s="14">
+        <v>4</v>
+      </c>
       <c r="N24" s="12"/>
       <c r="O24" s="12"/>
       <c r="P24" s="15"/>
@@ -1789,9 +1844,11 @@
       </c>
       <c r="L25" s="9">
         <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="M25" s="14"/>
+        <v>0</v>
+      </c>
+      <c r="M25" s="14">
+        <v>4</v>
+      </c>
       <c r="N25" s="12"/>
       <c r="O25" s="12"/>
       <c r="P25" s="15"/>
@@ -1829,7 +1886,9 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="M26" s="14"/>
+      <c r="M26" s="14">
+        <v>0</v>
+      </c>
       <c r="N26" s="12"/>
       <c r="O26" s="12"/>
       <c r="P26" s="15"/>
@@ -1865,10 +1924,14 @@
       </c>
       <c r="L27" s="9">
         <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="M27" s="14"/>
-      <c r="N27" s="12"/>
+        <v>0</v>
+      </c>
+      <c r="M27" s="14">
+        <v>0</v>
+      </c>
+      <c r="N27" s="12">
+        <v>4</v>
+      </c>
       <c r="O27" s="12"/>
       <c r="P27" s="15"/>
     </row>
@@ -1905,8 +1968,12 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="M28" s="14"/>
-      <c r="N28" s="12"/>
+      <c r="M28" s="14">
+        <v>0</v>
+      </c>
+      <c r="N28" s="12">
+        <v>0</v>
+      </c>
       <c r="O28" s="12"/>
       <c r="P28" s="15"/>
     </row>
@@ -1943,7 +2010,9 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="M29" s="14"/>
+      <c r="M29" s="14">
+        <v>0</v>
+      </c>
       <c r="N29" s="12"/>
       <c r="O29" s="12"/>
       <c r="P29" s="15"/>
@@ -1981,7 +2050,9 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="M30" s="14"/>
+      <c r="M30" s="14">
+        <v>0</v>
+      </c>
       <c r="N30" s="12"/>
       <c r="O30" s="12"/>
       <c r="P30" s="15"/>
@@ -2019,7 +2090,9 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="M31" s="14"/>
+      <c r="M31" s="14">
+        <v>0</v>
+      </c>
       <c r="N31" s="12"/>
       <c r="O31" s="12"/>
       <c r="P31" s="15"/>
@@ -2057,7 +2130,9 @@
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="M32" s="14"/>
+      <c r="M32" s="14">
+        <v>0</v>
+      </c>
       <c r="N32" s="12"/>
       <c r="O32" s="12"/>
       <c r="P32" s="15"/>
@@ -2095,7 +2170,9 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="M33" s="14"/>
+      <c r="M33" s="14">
+        <v>0</v>
+      </c>
       <c r="N33" s="12"/>
       <c r="O33" s="12"/>
       <c r="P33" s="15"/>
@@ -2131,9 +2208,11 @@
       </c>
       <c r="L34" s="9">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="M34" s="14"/>
+        <v>0</v>
+      </c>
+      <c r="M34" s="14">
+        <v>2</v>
+      </c>
       <c r="N34" s="12"/>
       <c r="O34" s="12"/>
       <c r="P34" s="15"/>
@@ -2169,9 +2248,11 @@
       </c>
       <c r="L35" s="9">
         <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="M35" s="14"/>
+        <v>2</v>
+      </c>
+      <c r="M35" s="14">
+        <v>2</v>
+      </c>
       <c r="N35" s="12"/>
       <c r="O35" s="12"/>
       <c r="P35" s="15"/>
@@ -2207,9 +2288,11 @@
       </c>
       <c r="L36" s="9">
         <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="M36" s="14"/>
+        <v>3</v>
+      </c>
+      <c r="M36" s="14">
+        <v>1</v>
+      </c>
       <c r="N36" s="12"/>
       <c r="O36" s="12"/>
       <c r="P36" s="15"/>
@@ -2243,18 +2326,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="M5:P5"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="K5:K6"/>
+    <mergeCell ref="L5:L6"/>
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="D5:D6"/>
     <mergeCell ref="E5:E6"/>
     <mergeCell ref="F5:F6"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="K5:K6"/>
-    <mergeCell ref="L5:L6"/>
-    <mergeCell ref="M5:P5"/>
-    <mergeCell ref="G5:G6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Se anezan documentos SPRINT 2
</commit_message>
<xml_diff>
--- a/SPRINT 1/1-Planificacion/Pila del Sprint/Pila General del Sprint 1.xlsx
+++ b/SPRINT 1/1-Planificacion/Pila del Sprint/Pila General del Sprint 1.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="76">
   <si>
     <t>ID</t>
   </si>
@@ -176,9 +176,6 @@
     <t>SEGUNDA REVISION DE CALIDAD</t>
   </si>
   <si>
-    <t>LECTURAS DE DOCUMENTOS DE DESARROLLO</t>
-  </si>
-  <si>
     <t>SCRUM MASTER</t>
   </si>
   <si>
@@ -200,9 +197,6 @@
     <t>EQUIPO</t>
   </si>
   <si>
-    <t>LIBROS, WEB</t>
-  </si>
-  <si>
     <t>DOCUMENTO</t>
   </si>
   <si>
@@ -219,9 +213,6 @@
   </si>
   <si>
     <t>REPOSITORIO</t>
-  </si>
-  <si>
-    <t>INFORME</t>
   </si>
   <si>
     <t>FINAL DEL SPRINT</t>
@@ -278,7 +269,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -653,46 +644,46 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -974,11 +965,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:P46"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B1:P45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M33" sqref="M33"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35:XFD35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -1033,57 +1024,57 @@
     </row>
     <row r="4" spans="2:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B5" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="22" t="s">
+      <c r="B5" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="E5" s="22" t="s">
+      <c r="D5" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="G5" s="22" t="s">
+      <c r="F5" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="H5" s="26" t="s">
+      <c r="H5" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="I5" s="26" t="s">
+      <c r="I5" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="J5" s="29" t="s">
+      <c r="J5" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="K5" s="24" t="s">
+      <c r="K5" s="28" t="s">
         <v>8</v>
       </c>
       <c r="L5" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="M5" s="32" t="s">
+      <c r="M5" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="N5" s="22"/>
-      <c r="O5" s="22"/>
-      <c r="P5" s="33"/>
+      <c r="N5" s="21"/>
+      <c r="O5" s="21"/>
+      <c r="P5" s="22"/>
     </row>
     <row r="6" spans="2:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="21"/>
+      <c r="B6" s="33"/>
       <c r="C6" s="23"/>
       <c r="D6" s="23"/>
       <c r="E6" s="23"/>
-      <c r="F6" s="25"/>
+      <c r="F6" s="29"/>
       <c r="G6" s="23"/>
-      <c r="H6" s="27"/>
-      <c r="I6" s="28"/>
-      <c r="J6" s="27"/>
-      <c r="K6" s="25"/>
+      <c r="H6" s="25"/>
+      <c r="I6" s="26"/>
+      <c r="J6" s="25"/>
+      <c r="K6" s="29"/>
       <c r="L6" s="31"/>
       <c r="M6" s="2" t="s">
         <v>11</v>
@@ -1110,19 +1101,19 @@
         <v>37</v>
       </c>
       <c r="F7" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="G7" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="G7" s="6" t="s">
-        <v>48</v>
-      </c>
       <c r="H7" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="J7" s="8" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="K7" s="6">
         <v>2</v>
@@ -1148,25 +1139,25 @@
         <v>37</v>
       </c>
       <c r="F8" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="G8" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="G8" s="6" t="s">
-        <v>48</v>
-      </c>
       <c r="H8" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="J8" s="8" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="K8" s="6">
         <v>2</v>
       </c>
       <c r="L8" s="9">
-        <f t="shared" ref="L8:L36" si="0">K8-(SUM(M8:P8))</f>
+        <f t="shared" ref="L8:L35" si="0">K8-(SUM(M8:P8))</f>
         <v>2</v>
       </c>
       <c r="M8" s="10"/>
@@ -1186,19 +1177,19 @@
         <v>37</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="J9" s="8" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="K9" s="6">
         <v>8</v>
@@ -1228,19 +1219,19 @@
         <v>38</v>
       </c>
       <c r="F10" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="G10" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="G10" s="6" t="s">
-        <v>48</v>
-      </c>
       <c r="H10" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="J10" s="8" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="K10" s="6">
         <v>8</v>
@@ -1270,19 +1261,19 @@
         <v>38</v>
       </c>
       <c r="F11" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="G11" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="G11" s="6" t="s">
-        <v>48</v>
-      </c>
       <c r="H11" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="J11" s="8" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="K11" s="6">
         <v>8</v>
@@ -1315,16 +1306,16 @@
         <v>40</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I12" s="7">
         <v>42959</v>
       </c>
       <c r="J12" s="8" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="K12" s="6">
         <v>10</v>
@@ -1346,7 +1337,7 @@
         <v>23</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E13" s="12" t="s">
         <v>39</v>
@@ -1355,16 +1346,16 @@
         <v>40</v>
       </c>
       <c r="G13" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H13" s="12" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I13" s="16">
         <v>42959</v>
       </c>
       <c r="J13" s="8" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="K13" s="12">
         <v>4</v>
@@ -1388,7 +1379,7 @@
         <v>23</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E14" s="12" t="s">
         <v>39</v>
@@ -1400,13 +1391,13 @@
         <v>15</v>
       </c>
       <c r="H14" s="12" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I14" s="7">
         <v>42959</v>
       </c>
       <c r="J14" s="8" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="K14" s="12">
         <v>4</v>
@@ -1436,19 +1427,19 @@
         <v>39</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G15" s="12" t="s">
         <v>15</v>
       </c>
       <c r="H15" s="12" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I15" s="7">
         <v>42960</v>
       </c>
       <c r="J15" s="13" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="K15" s="12">
         <v>4</v>
@@ -1468,7 +1459,7 @@
       <c r="B16" s="5"/>
       <c r="C16" s="6"/>
       <c r="D16" s="12" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E16" s="12"/>
       <c r="F16" s="6"/>
@@ -1480,7 +1471,7 @@
         <v>42964</v>
       </c>
       <c r="J16" s="13" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="K16" s="12">
         <v>4</v>
@@ -1504,7 +1495,7 @@
         <v>23</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E17" s="12" t="s">
         <v>39</v>
@@ -1516,13 +1507,13 @@
         <v>15</v>
       </c>
       <c r="H17" s="12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I17" s="7">
         <v>42961</v>
       </c>
       <c r="J17" s="13" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="K17" s="12">
         <v>4</v>
@@ -1544,11 +1535,11 @@
       <c r="B18" s="5"/>
       <c r="C18" s="6"/>
       <c r="D18" s="12" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E18" s="12"/>
       <c r="F18" s="6" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G18" s="12" t="s">
         <v>15</v>
@@ -1558,7 +1549,7 @@
         <v>42962</v>
       </c>
       <c r="J18" s="13" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="K18" s="12">
         <v>4</v>
@@ -1582,11 +1573,11 @@
         <v>23</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E19" s="12"/>
       <c r="F19" s="6" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G19" s="12" t="s">
         <v>15</v>
@@ -1596,7 +1587,7 @@
         <v>42963</v>
       </c>
       <c r="J19" s="13" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="K19" s="12">
         <v>4</v>
@@ -1626,19 +1617,19 @@
         <v>39</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G20" s="12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H20" s="12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="I20" s="7">
         <v>42969</v>
       </c>
       <c r="J20" s="13" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="K20" s="12">
         <v>6</v>
@@ -1665,19 +1656,19 @@
         <v>38</v>
       </c>
       <c r="F21" s="12" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G21" s="12" t="s">
         <v>15</v>
       </c>
       <c r="H21" s="12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I21" s="7">
         <v>42970</v>
       </c>
       <c r="J21" s="13" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="K21" s="12">
         <v>16</v>
@@ -1705,19 +1696,19 @@
         <v>39</v>
       </c>
       <c r="F22" s="12" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G22" s="12" t="s">
         <v>15</v>
       </c>
       <c r="H22" s="12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I22" s="7">
         <v>42970</v>
       </c>
       <c r="J22" s="13" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="K22" s="12">
         <v>16</v>
@@ -1745,19 +1736,19 @@
         <v>39</v>
       </c>
       <c r="F23" s="12" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G23" s="12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H23" s="12" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="I23" s="7">
         <v>42970</v>
       </c>
       <c r="J23" s="13" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="K23" s="12">
         <v>4</v>
@@ -1785,19 +1776,19 @@
         <v>38</v>
       </c>
       <c r="F24" s="12" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G24" s="12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H24" s="12" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="I24" s="16">
         <v>42966</v>
       </c>
       <c r="J24" s="13" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="K24" s="12">
         <v>4</v>
@@ -1819,25 +1810,25 @@
         <v>29</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E25" s="12" t="s">
         <v>38</v>
       </c>
       <c r="F25" s="12" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G25" s="12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H25" s="12" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="I25" s="16">
         <v>42971</v>
       </c>
       <c r="J25" s="13" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="K25" s="12">
         <v>4</v>
@@ -1865,19 +1856,19 @@
         <v>38</v>
       </c>
       <c r="F26" s="12" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G26" s="12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H26" s="12" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="I26" s="16">
         <v>42973</v>
       </c>
       <c r="J26" s="13" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="K26" s="12">
         <v>4</v>
@@ -1899,25 +1890,25 @@
         <v>29</v>
       </c>
       <c r="D27" s="12" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E27" s="12" t="s">
         <v>39</v>
       </c>
       <c r="F27" s="12" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G27" s="12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H27" s="12" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="I27" s="16">
         <v>42973</v>
       </c>
       <c r="J27" s="13" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="K27" s="12">
         <v>4</v>
@@ -1941,25 +1932,25 @@
         <v>29</v>
       </c>
       <c r="D28" s="12" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E28" s="12" t="s">
         <v>39</v>
       </c>
       <c r="F28" s="12" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G28" s="12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H28" s="12" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="I28" s="16">
         <v>42976</v>
       </c>
       <c r="J28" s="13" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="K28" s="12">
         <v>4</v>
@@ -1983,7 +1974,7 @@
         <v>33</v>
       </c>
       <c r="D29" s="12" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E29" s="12" t="s">
         <v>39</v>
@@ -1992,16 +1983,16 @@
         <v>40</v>
       </c>
       <c r="G29" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H29" s="12" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I29" s="16">
         <v>42977</v>
       </c>
       <c r="J29" s="13" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="K29" s="12">
         <v>2</v>
@@ -2023,7 +2014,7 @@
         <v>33</v>
       </c>
       <c r="D30" s="12" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E30" s="12" t="s">
         <v>38</v>
@@ -2032,16 +2023,16 @@
         <v>40</v>
       </c>
       <c r="G30" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H30" s="12" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I30" s="16">
         <v>42977</v>
       </c>
       <c r="J30" s="13" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="K30" s="12">
         <v>2</v>
@@ -2063,7 +2054,7 @@
         <v>33</v>
       </c>
       <c r="D31" s="12" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E31" s="12" t="s">
         <v>38</v>
@@ -2072,16 +2063,16 @@
         <v>40</v>
       </c>
       <c r="G31" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H31" s="12" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I31" s="16">
         <v>42977</v>
       </c>
       <c r="J31" s="13" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="K31" s="12">
         <v>2</v>
@@ -2112,16 +2103,16 @@
         <v>40</v>
       </c>
       <c r="G32" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H32" s="12" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I32" s="16" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="J32" s="13" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="K32" s="12">
         <v>16</v>
@@ -2149,19 +2140,19 @@
         <v>39</v>
       </c>
       <c r="F33" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G33" s="12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H33" s="12" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="I33" s="16">
         <v>42977</v>
       </c>
       <c r="J33" s="13" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="K33" s="12">
         <v>2</v>
@@ -2189,19 +2180,19 @@
         <v>39</v>
       </c>
       <c r="F34" s="12" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G34" s="12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H34" s="12" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I34" s="16">
         <v>42959</v>
       </c>
       <c r="J34" s="8" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="K34" s="12">
         <v>2</v>
@@ -2223,85 +2214,48 @@
         <v>43</v>
       </c>
       <c r="D35" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E35" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F35" s="12" t="s">
         <v>40</v>
       </c>
       <c r="G35" s="12" t="s">
-        <v>54</v>
+        <v>2</v>
       </c>
       <c r="H35" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="I35" s="16">
-        <v>42797</v>
+        <v>41</v>
+      </c>
+      <c r="I35" s="16" t="s">
+        <v>60</v>
       </c>
       <c r="J35" s="13" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="K35" s="12">
         <v>4</v>
       </c>
       <c r="L35" s="9">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M35" s="14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N35" s="12"/>
       <c r="O35" s="12"/>
       <c r="P35" s="15"/>
     </row>
-    <row r="36" spans="2:16" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B36" s="5"/>
-      <c r="C36" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="D36" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="E36" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="F36" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="G36" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="H36" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="I36" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="J36" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="K36" s="12">
-        <v>4</v>
-      </c>
-      <c r="L36" s="9">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="M36" s="14">
-        <v>1</v>
-      </c>
-      <c r="N36" s="12"/>
-      <c r="O36" s="12"/>
-      <c r="P36" s="15"/>
+    <row r="38" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C38" s="17"/>
+      <c r="D38" s="18"/>
+      <c r="J38" s="17"/>
+      <c r="L38" s="17"/>
     </row>
     <row r="39" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="C39" s="17"/>
       <c r="D39" s="18"/>
-      <c r="J39" s="17"/>
-      <c r="L39" s="17"/>
     </row>
     <row r="40" spans="2:16" x14ac:dyDescent="0.25">
       <c r="D40" s="18"/>
@@ -2321,11 +2275,13 @@
     <row r="45" spans="2:16" x14ac:dyDescent="0.25">
       <c r="D45" s="18"/>
     </row>
-    <row r="46" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="D46" s="18"/>
-    </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:F6"/>
     <mergeCell ref="M5:P5"/>
     <mergeCell ref="G5:G6"/>
     <mergeCell ref="H5:H6"/>
@@ -2333,11 +2289,6 @@
     <mergeCell ref="J5:J6"/>
     <mergeCell ref="K5:K6"/>
     <mergeCell ref="L5:L6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F5:F6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>